<commit_message>
last version of the project (start testing, prepare deploy)
</commit_message>
<xml_diff>
--- a/media/temp_files/invoice.xlsx
+++ b/media/temp_files/invoice.xlsx
@@ -619,7 +619,7 @@
       <c r="A2" s="37" t="n"/>
       <c r="H2" s="9" t="inlineStr">
         <is>
-          <t>0000000004</t>
+          <t>0000000003</t>
         </is>
       </c>
       <c r="I2" s="10" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="J2" s="38" t="inlineStr">
         <is>
-          <t>0000000003</t>
+          <t>0000000005</t>
         </is>
       </c>
       <c r="K2" s="39" t="n"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="B5" s="15" t="inlineStr">
         <is>
-          <t>Яничева Галина Яничева, ул.  Большая Арнаутская, 26, квартира № 31</t>
+          <t>Карпов Николай Карпов, ул.  Большая Арнаутская, 26, квартира № 7</t>
         </is>
       </c>
       <c r="H5" s="14" t="n"/>
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="B6" s="16" t="n">
-        <v>1120</v>
+        <v>600</v>
       </c>
       <c r="C6" s="14" t="n"/>
       <c r="D6" s="14" t="n"/>
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="B7" s="16" t="n">
-        <v>2000</v>
+        <v>-200</v>
       </c>
       <c r="C7" s="17" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="B8" s="16" t="n">
-        <v>1120</v>
+        <v>600</v>
       </c>
       <c r="C8" s="17" t="inlineStr">
         <is>
@@ -918,7 +918,7 @@
       <c r="A11" s="37" t="n"/>
       <c r="H11" s="9" t="inlineStr">
         <is>
-          <t>0000000004</t>
+          <t>0000000003</t>
         </is>
       </c>
       <c r="I11" s="10" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="J11" s="38" t="inlineStr">
         <is>
-          <t>0000000003</t>
+          <t>0000000005</t>
         </is>
       </c>
       <c r="K11" s="39" t="n"/>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B14" s="15" t="inlineStr">
         <is>
-          <t>Яничева Галина Яничева, ул.  Большая Арнаутская, 26, квартира № 31</t>
+          <t>Карпов Николай Карпов, ул.  Большая Арнаутская, 26, квартира № 7</t>
         </is>
       </c>
       <c r="H14" s="14" t="n"/>
@@ -1038,7 +1038,7 @@
         </is>
       </c>
       <c r="B15" s="16" t="n">
-        <v>1120</v>
+        <v>600</v>
       </c>
       <c r="C15" s="14" t="n"/>
       <c r="D15" s="14" t="n"/>
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B16" s="16" t="n">
-        <v>2000</v>
+        <v>-200</v>
       </c>
       <c r="C16" s="17" t="inlineStr">
         <is>
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="B17" s="16" t="n">
-        <v>1120</v>
+        <v>600</v>
       </c>
       <c r="C17" s="17" t="inlineStr">
         <is>
@@ -1213,11 +1213,11 @@
       </c>
       <c r="F19" s="46" t="n"/>
       <c r="G19" s="46" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H19" s="46" t="n"/>
       <c r="I19" s="46" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J19" s="46" t="n"/>
       <c r="K19" s="44" t="n"/>
@@ -1255,11 +1255,11 @@
       </c>
       <c r="F20" s="46" t="n"/>
       <c r="G20" s="46" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H20" s="46" t="n"/>
       <c r="I20" s="46" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="J20" s="46" t="n"/>
       <c r="L20" s="7" t="n"/>
@@ -1296,11 +1296,11 @@
       </c>
       <c r="F21" s="46" t="n"/>
       <c r="G21" s="46" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H21" s="46" t="n"/>
       <c r="I21" s="46" t="n">
-        <v>900</v>
+        <v>300</v>
       </c>
       <c r="J21" s="46" t="n"/>
       <c r="L21" s="7" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="H22" s="46" t="n"/>
       <c r="I22" s="46" t="n">
-        <v>1120</v>
+        <v>600</v>
       </c>
       <c r="J22" s="46" t="n"/>
       <c r="L22" s="7" t="n"/>

</xml_diff>